<commit_message>
para hacer pruebas en la mac
</commit_message>
<xml_diff>
--- a/Codes/Tesis/LocalSearch/CoordenadasAccidentes.xlsx
+++ b/Codes/Tesis/LocalSearch/CoordenadasAccidentes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beatr\Documents\EstudiosProfesionales\FIME\Doctorado\TesisDoctoral\Codes\Tesis\LocalSearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B6D01D-617C-4505-B267-5F4176B24859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F765F4-B2F2-4CA8-BF7C-E97E17C093B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="6" xr2:uid="{81BBF99F-1DB1-49E1-9BE7-28ADF641FF4B}"/>
   </bookViews>
@@ -90499,9 +90499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{306DD0B8-17F4-4818-B672-9970267E1545}">
   <dimension ref="B2:C653"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>